<commit_message>
version sent to adeel with a few holes
</commit_message>
<xml_diff>
--- a/results/SpeedGraphs.xlsx
+++ b/results/SpeedGraphs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15560" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="8280" yWindow="20" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,6 +149,29 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Demarcation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Speed</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
@@ -156,10 +179,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0550597078506548"/>
-          <c:y val="0.0159574468085106"/>
+          <c:x val="0.130982578519967"/>
+          <c:y val="0.0599455040871934"/>
           <c:w val="0.7838467246568"/>
-          <c:h val="0.898014324007371"/>
+          <c:h val="0.816270462786157"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -343,6 +366,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -352,7 +380,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0243883105215875"/>
+                  <c:y val="0.0600725181831834"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -523,11 +556,16 @@
           <c:trendline>
             <c:trendlineType val="poly"/>
             <c:order val="3"/>
-            <c:forward val="1.5"/>
+            <c:forward val="0.5"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0225538586200215"/>
+                  <c:y val="0.171662125340599"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -594,21 +632,40 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2122037864"/>
-        <c:axId val="2121885816"/>
+        <c:axId val="2085273000"/>
+        <c:axId val="2085275736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2122037864"/>
+        <c:axId val="2085273000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Input size (nu)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121885816"/>
+        <c:crossAx val="2085275736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -616,23 +673,48 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2121885816"/>
+        <c:axId val="2085275736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Run</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122037864"/>
+        <c:crossAx val="2085273000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:legendEntry>
         <c:idx val="5"/>
         <c:delete val="1"/>
@@ -641,13 +723,27 @@
         <c:idx val="6"/>
         <c:delete val="1"/>
       </c:legendEntry>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0872581866863957"/>
+          <c:y val="0.107901907356948"/>
+          <c:w val="0.653224118797231"/>
+          <c:h val="0.054721834838765"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -660,16 +756,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>